<commit_message>
Bulk insert and doc
</commit_message>
<xml_diff>
--- a/Progress Reports/CDC Monthly progress reports/2016/CDC RIF plans - July 2016 to March 2017.xlsx
+++ b/Progress Reports/CDC Monthly progress reports/2016/CDC RIF plans - July 2016 to March 2017.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="239">
   <si>
     <t>Details</t>
   </si>
@@ -751,9 +751,6 @@
     <t>Not allocated (for overrun - 10 days): now data viewer get methods</t>
   </si>
   <si>
-    <t>SQL Server study submission and data extraction</t>
-  </si>
-  <si>
     <t>CDC Visit</t>
   </si>
   <si>
@@ -772,13 +769,22 @@
     <t>SQL Server middleware</t>
   </si>
   <si>
-    <t>Reamaining data display methods</t>
-  </si>
-  <si>
     <t>SQL Server tile integration</t>
   </si>
   <si>
     <t>Non RIF activities</t>
+  </si>
+  <si>
+    <t>Java handover</t>
+  </si>
+  <si>
+    <t>Java handover, fix submission failures</t>
+  </si>
+  <si>
+    <t>Reamaining data display methods, Java</t>
+  </si>
+  <si>
+    <t>SQL Server study submission and data extraction; installer documentation</t>
   </si>
 </sst>
 </file>
@@ -865,7 +871,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1007,30 +1013,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2570,11 +2589,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12:F27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2623,7 +2642,7 @@
         <f>DATE(2016,1,-2)-WEEKDAY(DATE(2016,1,3))+A3*7</f>
         <v>42555</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="50" t="s">
         <v>178</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -2632,7 +2651,7 @@
       <c r="E3" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="55" t="s">
         <v>182</v>
       </c>
       <c r="G3" s="32"/>
@@ -2646,11 +2665,11 @@
         <f t="shared" ref="B4:B28" si="0">DATE(2016,1,-2)-WEEKDAY(DATE(2016,1,3))+A4*7</f>
         <v>42562</v>
       </c>
-      <c r="C4" s="44"/>
+      <c r="C4" s="50"/>
       <c r="E4" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="F4" s="48"/>
+      <c r="F4" s="55"/>
       <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -2662,17 +2681,17 @@
         <f t="shared" si="0"/>
         <v>42569</v>
       </c>
-      <c r="C5" s="44"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="34" t="s">
         <v>211</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="G5" s="48"/>
+      <c r="G5" s="55"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="37">
@@ -2683,15 +2702,15 @@
         <f t="shared" si="0"/>
         <v>42576</v>
       </c>
-      <c r="C6" s="44"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="21" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="40" t="s">
         <v>213</v>
       </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="48"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="6" t="s">
         <v>74</v>
       </c>
@@ -2705,19 +2724,19 @@
         <f t="shared" si="0"/>
         <v>42583</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="50" t="s">
         <v>182</v>
       </c>
       <c r="E7" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="G7" s="48"/>
+      <c r="G7" s="55"/>
     </row>
     <row r="8" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="37">
@@ -2728,13 +2747,13 @@
         <f t="shared" si="0"/>
         <v>42590</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="48"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="55"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="37">
@@ -2748,16 +2767,16 @@
       <c r="C9" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="50" t="s">
         <v>220</v>
       </c>
       <c r="E9" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="G9" s="48"/>
+      <c r="G9" s="55"/>
     </row>
     <row r="10" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="37">
@@ -2771,12 +2790,12 @@
       <c r="C10" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="50"/>
       <c r="E10" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="F10" s="49"/>
-      <c r="G10" s="48"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="55"/>
     </row>
     <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="37">
@@ -2787,10 +2806,10 @@
         <f t="shared" si="0"/>
         <v>42611</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="50" t="s">
         <v>201</v>
       </c>
-      <c r="D11" s="44"/>
+      <c r="D11" s="50"/>
       <c r="E11" s="27" t="s">
         <v>208</v>
       </c>
@@ -2813,14 +2832,14 @@
         <f t="shared" si="0"/>
         <v>42618</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="44" t="s">
+      <c r="C12" s="51"/>
+      <c r="D12" s="50" t="s">
         <v>226</v>
       </c>
       <c r="E12" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="F12" s="47" t="s">
+      <c r="F12" s="53" t="s">
         <v>209</v>
       </c>
       <c r="G12" s="21" t="s">
@@ -2836,15 +2855,15 @@
         <f t="shared" si="0"/>
         <v>42625</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="50" t="s">
         <v>200</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44" t="s">
+      <c r="D13" s="50"/>
+      <c r="E13" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="F13" s="45"/>
-      <c r="G13" s="44" t="s">
+      <c r="F13" s="51"/>
+      <c r="G13" s="50" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2857,13 +2876,13 @@
         <f t="shared" si="0"/>
         <v>42632</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="50" t="s">
+      <c r="C14" s="50"/>
+      <c r="D14" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="44"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="50"/>
       <c r="H14" s="6" t="s">
         <v>73</v>
       </c>
@@ -2877,13 +2896,13 @@
         <f t="shared" si="0"/>
         <v>42639</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="44"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="37">
@@ -2894,15 +2913,15 @@
         <f t="shared" si="0"/>
         <v>42646</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44" t="s">
-        <v>230</v>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50" t="s">
+        <v>229</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="44"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="37">
@@ -2913,15 +2932,15 @@
         <f t="shared" si="0"/>
         <v>42653</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="50" t="s">
         <v>225</v>
       </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="44" t="s">
+      <c r="D17" s="51"/>
+      <c r="E17" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="44"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="37">
@@ -2932,11 +2951,11 @@
         <f t="shared" si="0"/>
         <v>42660</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="44"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="50"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="37">
@@ -2947,11 +2966,11 @@
         <f t="shared" si="0"/>
         <v>42667</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="44"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="37">
@@ -2962,15 +2981,15 @@
         <f t="shared" si="0"/>
         <v>42674</v>
       </c>
-      <c r="C20" s="45"/>
+      <c r="C20" s="51"/>
       <c r="D20" s="39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E20" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="F20" s="46"/>
-      <c r="G20" s="44"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="37">
@@ -2981,17 +3000,17 @@
         <f t="shared" si="0"/>
         <v>42681</v>
       </c>
-      <c r="C21" s="45"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="41" t="s">
-        <v>229</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>232</v>
-      </c>
-      <c r="F21" s="46"/>
-      <c r="G21" s="44"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>228</v>
+      </c>
+      <c r="E21" s="50" t="s">
+        <v>231</v>
+      </c>
+      <c r="F21" s="54"/>
+      <c r="G21" s="50"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="37">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -3000,13 +3019,15 @@
         <f t="shared" si="0"/>
         <v>42688</v>
       </c>
-      <c r="C22" s="45"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="E22" s="44"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="44"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="44" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="37">
@@ -3017,13 +3038,18 @@
         <f t="shared" si="0"/>
         <v>42695</v>
       </c>
-      <c r="C23" s="45"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="41" t="s">
-        <v>229</v>
-      </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="44"/>
+        <v>236</v>
+      </c>
+      <c r="E23" s="51"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="37">
@@ -3034,17 +3060,17 @@
         <f t="shared" si="0"/>
         <v>42702</v>
       </c>
-      <c r="C24" s="44" t="s">
-        <v>235</v>
-      </c>
-      <c r="D24" s="44" t="s">
+      <c r="C24" s="50" t="s">
+        <v>233</v>
+      </c>
+      <c r="D24" s="50" t="s">
         <v>221</v>
       </c>
       <c r="E24" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="44"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="55"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="37">
@@ -3055,15 +3081,13 @@
         <f t="shared" si="0"/>
         <v>42709</v>
       </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="48" t="s">
-        <v>234</v>
-      </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="48" t="s">
-        <v>233</v>
-      </c>
+      <c r="C25" s="50"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="55" t="s">
+        <v>237</v>
+      </c>
+      <c r="F25" s="54"/>
+      <c r="G25" s="55"/>
     </row>
     <row r="26" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="37">
@@ -3074,11 +3098,11 @@
         <f t="shared" si="0"/>
         <v>42716</v>
       </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="48"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="55"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="37">
@@ -3092,10 +3116,10 @@
       <c r="C27" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="D27" s="45"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="48"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="55"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="37">
@@ -3106,36 +3130,36 @@
         <f t="shared" si="0"/>
         <v>42730</v>
       </c>
-      <c r="C28" s="53" t="s">
+      <c r="C28" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
     </row>
     <row r="29" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="37">
         <v>1</v>
       </c>
       <c r="B29" s="38">
-        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A29*7</f>
+        <f t="shared" ref="B29:B42" si="2">DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A29*7</f>
         <v>42737</v>
       </c>
-      <c r="C29" s="44" t="s">
-        <v>227</v>
-      </c>
-      <c r="D29" s="44" t="s">
+      <c r="C29" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="D29" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="55" t="s">
         <v>224</v>
       </c>
-      <c r="F29" s="54"/>
-      <c r="G29" s="48" t="s">
-        <v>233</v>
+      <c r="F29" s="56"/>
+      <c r="G29" s="47" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -3143,42 +3167,42 @@
         <v>2</v>
       </c>
       <c r="B30" s="38">
-        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A30*7</f>
+        <f t="shared" si="2"/>
         <v>42744</v>
       </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="48"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="47"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="37">
         <v>3</v>
       </c>
       <c r="B31" s="38">
-        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A31*7</f>
+        <f t="shared" si="2"/>
         <v>42751</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="48"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="47"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="37">
         <v>4</v>
       </c>
       <c r="B32" s="38">
-        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A32*7</f>
+        <f t="shared" si="2"/>
         <v>42758</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="48"/>
       <c r="H32" s="6" t="s">
         <v>72</v>
       </c>
@@ -3188,16 +3212,16 @@
         <v>5</v>
       </c>
       <c r="B33" s="38">
-        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A33*7</f>
+        <f t="shared" si="2"/>
         <v>42765</v>
       </c>
-      <c r="C33" s="44"/>
+      <c r="C33" s="50"/>
       <c r="D33" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="48"/>
       <c r="H33" s="6" t="s">
         <v>71</v>
       </c>
@@ -3207,39 +3231,41 @@
         <v>6</v>
       </c>
       <c r="B34" s="38">
-        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A34*7</f>
+        <f t="shared" si="2"/>
         <v>42772</v>
       </c>
-      <c r="C34" s="51" t="s">
-        <v>228</v>
-      </c>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="54"/>
+      <c r="C34" s="57" t="s">
+        <v>227</v>
+      </c>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="37">
         <v>7</v>
       </c>
       <c r="B35" s="38">
-        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A35*7</f>
+        <f t="shared" si="2"/>
         <v>42779</v>
       </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="37">
         <v>8</v>
       </c>
       <c r="B36" s="38">
-        <f>DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A36*7</f>
+        <f t="shared" si="2"/>
         <v>42786</v>
       </c>
       <c r="C36" s="42"/>
@@ -3249,30 +3275,108 @@
       <c r="G36" s="43"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D37" s="27"/>
+      <c r="A37" s="37">
+        <v>9</v>
+      </c>
+      <c r="B37" s="38">
+        <f t="shared" si="2"/>
+        <v>42793</v>
+      </c>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C38" s="21" t="s">
+      <c r="A38" s="37">
+        <v>10</v>
+      </c>
+      <c r="B38" s="38">
+        <f t="shared" si="2"/>
+        <v>42800</v>
+      </c>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="37">
+        <v>11</v>
+      </c>
+      <c r="B39" s="38">
+        <f t="shared" si="2"/>
+        <v>42807</v>
+      </c>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="37">
+        <v>12</v>
+      </c>
+      <c r="B40" s="38">
+        <f t="shared" si="2"/>
+        <v>42814</v>
+      </c>
+      <c r="D40" s="27"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="37">
+        <v>13</v>
+      </c>
+      <c r="B41" s="38">
+        <f t="shared" si="2"/>
+        <v>42821</v>
+      </c>
+      <c r="C41" s="45"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="37">
+        <v>14</v>
+      </c>
+      <c r="B42" s="38">
+        <f t="shared" si="2"/>
+        <v>42828</v>
+      </c>
+      <c r="C42" s="45"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C43" s="45"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C44" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="D38" s="39" t="s">
-        <v>236</v>
+      <c r="D44" s="39" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="C17:C23"/>
-    <mergeCell ref="F12:F27"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="G29:G33"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="E29:F33"/>
-    <mergeCell ref="C34:I34"/>
+  <mergeCells count="30">
+    <mergeCell ref="C34:I35"/>
+    <mergeCell ref="G5:G10"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G13:G21"/>
     <mergeCell ref="C29:C33"/>
     <mergeCell ref="E13:E15"/>
     <mergeCell ref="C28:I28"/>
@@ -3287,11 +3391,16 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="G13:G24"/>
-    <mergeCell ref="G5:G10"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F12:F27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="E29:F33"/>
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="C17:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>